<commit_message>
Se corrige el cu-16 visualizar avisos, se realizan correcciones en promociones y grupos
</commit_message>
<xml_diff>
--- a/Plantillas/Iteracion 6/Plantilla Lista de Tareas de la Iteracion iteracion 6 Fin.xlsx
+++ b/Plantillas/Iteracion 6/Plantilla Lista de Tareas de la Iteracion iteracion 6 Fin.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enriq\Documents\6TO SEMESTRE IS\DESARROLLO SOFTWARE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enriq\Documents\6TO SEMESTRE IS\DESARROLLO SOFTWARE\Proyecto\EMA-Desarrollo-de-software-Equipo-2\Plantillas\Iteracion 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -929,10 +929,10 @@
   <dimension ref="A1:BB218"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G144" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="Q124" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AU168" sqref="AU168"/>
+      <selection pane="bottomRight" activeCell="C127" sqref="C127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12753,8 +12753,8 @@
         <v>0</v>
       </c>
       <c r="BB86" s="13">
-        <f>SUM(AZ86:AZ91)</f>
-        <v>3.5</v>
+        <f>SUM(AZ86:AZ95)</f>
+        <v>21.5</v>
       </c>
     </row>
     <row r="87" spans="2:54" s="13" customFormat="1" ht="64.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -15754,8 +15754,8 @@
         <v>0</v>
       </c>
       <c r="BB107" s="13">
-        <f>SUM(AZ107:AZ112)</f>
-        <v>3.5</v>
+        <f>SUM(AZ107:AZ116)</f>
+        <v>22.5</v>
       </c>
     </row>
     <row r="108" spans="2:54" s="13" customFormat="1" ht="48.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17186,8 +17186,8 @@
         <v>0</v>
       </c>
       <c r="BB117" s="17">
-        <f>SUM(AZ117:AZ122)</f>
-        <v>3.5</v>
+        <f>SUM(AZ117:AZ126)</f>
+        <v>22.5</v>
       </c>
     </row>
     <row r="118" spans="2:54" s="17" customFormat="1" ht="65.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19686,8 +19686,8 @@
         <v>0</v>
       </c>
       <c r="BB137" s="17">
-        <f>SUM(AZ137:AZ142)</f>
-        <v>4.5</v>
+        <f>SUM(AZ137:AZ146)</f>
+        <v>20.5</v>
       </c>
     </row>
     <row r="138" spans="2:54" s="17" customFormat="1" ht="62.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -22695,8 +22695,8 @@
         <v>0</v>
       </c>
       <c r="BB158" s="21">
-        <f>SUM(AZ158:AZ163)</f>
-        <v>3</v>
+        <f>SUM(AZ158:AZ167)</f>
+        <v>16</v>
       </c>
     </row>
     <row r="159" spans="2:54" s="21" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -23835,11 +23835,12 @@
         <v>2</v>
       </c>
       <c r="AZ166" s="24">
-        <v>0</v>
+        <f t="shared" si="69"/>
+        <v>6</v>
       </c>
       <c r="BA166" s="24">
         <f t="shared" si="58"/>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="167" spans="2:54" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -23979,11 +23980,12 @@
         <v>1</v>
       </c>
       <c r="AZ167" s="24">
-        <v>0</v>
+        <f t="shared" si="69"/>
+        <v>2</v>
       </c>
       <c r="BA167" s="24">
         <f t="shared" si="58"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="2:54" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -30866,6 +30868,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -30877,11 +30884,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>